<commit_message>
Updated status to show Micha's completion of Joel review
</commit_message>
<xml_diff>
--- a/STATUS.xlsx
+++ b/STATUS.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS13\Desktop\Personal\Beis Journal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mo\Desktop\BEIS\Journal\BeisJournal25\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{46522D8D-3D97-4C4F-9895-6C434F0B937B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -299,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -468,7 +464,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -478,6 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -955,11 +951,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,11 +1790,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,10 +1835,10 @@
       <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E2" s="5"/>
@@ -1866,11 +1862,11 @@
         <v>64</v>
       </c>
       <c r="C3" s="7"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>68</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>74</v>
       </c>
       <c r="G3" s="8"/>
@@ -1891,7 +1887,7 @@
       <c r="B4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="8"/>
@@ -1918,10 +1914,10 @@
       <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>81</v>
       </c>
       <c r="E5" s="8"/>
@@ -1945,7 +1941,7 @@
       <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1976,17 +1972,17 @@
       <c r="B7" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
       <c r="K7">
         <f t="shared" si="1"/>
         <v>2</v>

</xml_diff>

<commit_message>
Updated status for recent developments
</commit_message>
<xml_diff>
--- a/STATUS.xlsx
+++ b/STATUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mo\Desktop\BEIS\Journal\BeisJournal25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{46522D8D-3D97-4C4F-9895-6C434F0B937B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22D54871-98A9-4758-800C-CBFFCED66B1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
   <si>
     <t>Surname</t>
   </si>
@@ -283,13 +283,13 @@
     <t>MS FINAL REVIEW?</t>
   </si>
   <si>
-    <t>Waiting for me</t>
-  </si>
-  <si>
     <t>Bordon</t>
   </si>
   <si>
     <t>Hallel acc Rambam</t>
+  </si>
+  <si>
+    <t>RabbiBordon</t>
   </si>
 </sst>
 </file>
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,8 +1112,8 @@
       <c r="G4" t="b">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>31</v>
+      <c r="H4" t="b">
+        <v>1</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -1436,8 +1436,8 @@
       <c r="G12" t="b">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
-        <v>31</v>
+      <c r="H12" t="b">
+        <v>1</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1491,7 +1491,7 @@
         <v>60</v>
       </c>
       <c r="L13" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1542,13 +1542,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
         <v>59</v>
@@ -1688,11 +1688,11 @@
       </c>
       <c r="G20" s="2">
         <f t="shared" ref="G20:J20" si="2">COUNTIF(G2:G19, "=TRUE")/COUNTA(C2:C19)</f>
-        <v>0.6470588235294118</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.47058823529411764</v>
+        <v>0.58823529411764708</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="2"/>
@@ -1793,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,7 +1844,9 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="K2">
         <v>2</v>
@@ -1944,7 +1946,7 @@
       <c r="C6" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="16" t="s">
         <v>72</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -1995,7 +1997,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9">
         <f>COUNTA(C2:I7)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to status for planning next few weeks of development
</commit_message>
<xml_diff>
--- a/STATUS.xlsx
+++ b/STATUS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mo\Desktop\BEIS\Journal\BeisJournal25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS13\Desktop\Personal\Beis Journal\BeisJournal25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22D54871-98A9-4758-800C-CBFFCED66B1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
   <si>
     <t>Surname</t>
   </si>
@@ -290,12 +290,78 @@
   </si>
   <si>
     <t>RabbiBordon</t>
+  </si>
+  <si>
+    <t>MS Sched</t>
+  </si>
+  <si>
+    <t>Complete Jsilv</t>
+  </si>
+  <si>
+    <t>Type up Jsilv</t>
+  </si>
+  <si>
+    <t>Page 1 MD</t>
+  </si>
+  <si>
+    <t>Page 2 MD</t>
+  </si>
+  <si>
+    <t>Page 3 MD</t>
+  </si>
+  <si>
+    <t>Page 4 MD</t>
+  </si>
+  <si>
+    <t>Complete MD</t>
+  </si>
+  <si>
+    <t>Computer MD</t>
+  </si>
+  <si>
+    <t>Section 1,2 SE</t>
+  </si>
+  <si>
+    <t>Section 3 SE</t>
+  </si>
+  <si>
+    <t>Section 4,5 SE</t>
+  </si>
+  <si>
+    <t>1/2 SE Computer</t>
+  </si>
+  <si>
+    <t>Final check of MK</t>
+  </si>
+  <si>
+    <t>2/2 SE Computer</t>
+  </si>
+  <si>
+    <t>1/2 Final check of DS</t>
+  </si>
+  <si>
+    <t>2/2 Final check of DS</t>
+  </si>
+  <si>
+    <t>Waiting on</t>
+  </si>
+  <si>
+    <t>Rabbi Bordon</t>
+  </si>
+  <si>
+    <t>As at 08/02/19</t>
+  </si>
+  <si>
+    <t>Rabbi Klein</t>
+  </si>
+  <si>
+    <t>Him</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +519,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -474,6 +540,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -951,11 +1018,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,11 +1857,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,4 +2070,317 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="20">
+        <v>43504</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(TEXT(C3, "dddd")="Saturday", "Motzash", TEXT(C3, "dddd"))</f>
+        <v>Friday</v>
+      </c>
+      <c r="I3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="20">
+        <v>43505</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D26" si="0">IF(TEXT(C4, "dddd")="Saturday", "Motzash", TEXT(C4, "dddd"))</f>
+        <v>Motzash</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="20">
+        <v>43506</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Sunday</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="20">
+        <v>43507</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Monday</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="20">
+        <v>43508</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="20">
+        <v>43509</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="20">
+        <v>43510</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Thursday</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="20">
+        <v>43511</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Friday</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="20">
+        <v>43512</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Motzash</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="20">
+        <v>43513</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sunday</v>
+      </c>
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="20">
+        <v>43514</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Monday</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="20">
+        <v>43515</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="20">
+        <v>43516</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="20">
+        <v>43517</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Thursday</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="20">
+        <v>43518</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Friday</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="20">
+        <v>43519</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Motzash</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="20">
+        <v>43520</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>Sunday</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="20">
+        <v>43521</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Monday</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="20">
+        <v>43522</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="20">
+        <v>43523</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Wednesday</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="20">
+        <v>43524</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Thursday</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="20">
+        <v>43525</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Friday</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="20">
+        <v>43526</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>Motzash</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="20">
+        <v>43527</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>Sunday</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of DSamole, almost complete, needs final review
</commit_message>
<xml_diff>
--- a/STATUS.xlsx
+++ b/STATUS.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="109">
   <si>
     <t>Surname</t>
   </si>
@@ -346,16 +346,13 @@
     <t>Waiting on</t>
   </si>
   <si>
-    <t>Rabbi Bordon</t>
-  </si>
-  <si>
-    <t>As at 08/02/19</t>
-  </si>
-  <si>
     <t>Rabbi Klein</t>
   </si>
   <si>
     <t>Him</t>
+  </si>
+  <si>
+    <t>As at 25/02/19</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1019,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -1621,7 +1618,7 @@
         <v>59</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1751,7 +1748,7 @@
       </c>
       <c r="F20" s="2">
         <f>COUNTIF(F2:F19, "=TRUE")/COUNTA(B2:B19)</f>
-        <v>0.82352941176470584</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" ref="G20:J20" si="2">COUNTIF(G2:G19, "=TRUE")/COUNTA(C2:C19)</f>
@@ -1759,7 +1756,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>0.6470588235294118</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="2"/>
@@ -2077,7 +2074,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,7 +2087,7 @@
         <v>88</v>
       </c>
       <c r="I1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2110,7 +2107,7 @@
         <v>106</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2123,12 +2120,6 @@
       </c>
       <c r="E4" t="s">
         <v>89</v>
-      </c>
-      <c r="I4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>